<commit_message>
Excel sheet looks into TA timing
</commit_message>
<xml_diff>
--- a/out2.xlsx
+++ b/out2.xlsx
@@ -21,16 +21,14 @@
     <sheet name="bug1079" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.0" hidden="1">'reducetestcase comment length'!$M$4:$M$145</definedName>
-    <definedName name="_xlchart.1" hidden="1">'reducetestcase comment length'!$L$3:$L$144</definedName>
-    <definedName name="_xlchart.2" hidden="1">'reducetestcase comment length'!$M$4:$M$145</definedName>
+    <definedName name="_xlchart.0" hidden="1">'reducetestcase comment length'!$L$3:$L$144</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4988" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5050" uniqueCount="878">
   <si>
     <t>collabid</t>
   </si>
@@ -2649,6 +2647,21 @@
   </si>
   <si>
     <t>Same grade</t>
+  </si>
+  <si>
+    <t>sum false</t>
+  </si>
+  <si>
+    <t>sum true</t>
+  </si>
+  <si>
+    <t>num rows</t>
+  </si>
+  <si>
+    <t>all her false's are at the end</t>
+  </si>
+  <si>
+    <t>somehow I don't believe these numbers</t>
   </si>
 </sst>
 </file>
@@ -2658,7 +2671,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2806,8 +2819,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3035,6 +3054,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -3211,7 +3236,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -3253,6 +3278,13 @@
     <xf numFmtId="0" fontId="19" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7133,7 +7165,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.1</cx:f>
+        <cx:f>_xlchart.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -10970,14 +11002,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T154"/>
   <sheetViews>
-    <sheetView topLeftCell="M26" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView topLeftCell="C127" workbookViewId="0">
+      <selection activeCell="M142" sqref="M142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" style="7" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="25.26953125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.36328125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.36328125" customWidth="1"/>
@@ -10989,6 +11022,9 @@
     <col min="13" max="13" width="22.54296875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="8.7265625" style="9"/>
+    <col min="16" max="16" width="9.453125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -11028,9 +11064,7 @@
         <f>CONCATENATE(K1, " ", L1)</f>
         <v>2018-03-07 11:36:51</v>
       </c>
-      <c r="R1" s="10" t="s">
-        <v>612</v>
-      </c>
+      <c r="R1" s="10"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
@@ -11073,10 +11107,6 @@
         <f>L2-L1</f>
         <v>4.9768518518522598E-4</v>
       </c>
-      <c r="R2" t="str">
-        <f>TEXT((P12+P34+P52+P70+P91+P111+P130+P149)/8, "hh:mm:ss")</f>
-        <v>00:00:49</v>
-      </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -11119,9 +11149,6 @@
         <f t="shared" ref="O3:O18" si="3">L3-L2</f>
         <v>1.2037037037036513E-3</v>
       </c>
-      <c r="R3" t="s">
-        <v>613</v>
-      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
@@ -11387,6 +11414,12 @@
       <c r="P9" s="10" t="s">
         <v>611</v>
       </c>
+      <c r="Q9" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -11430,8 +11463,16 @@
         <v>4.0509259259263741E-4</v>
       </c>
       <c r="P10" s="9" t="str">
-        <f>TEXT(SUM(O2:O18), "hh:mm:ss")</f>
-        <v>00:20:21</v>
+        <f>TEXT(SUM($O2:$O17), "hh:mm:ss")</f>
+        <v>00:13:28</v>
+      </c>
+      <c r="Q10" s="9" t="str">
+        <f>TEXT(SUMIF($D2:$D17, FALSE, $O2:$O17), "hh:mm:ss")</f>
+        <v>00:10:36</v>
+      </c>
+      <c r="R10" s="9" t="str">
+        <f>TEXT(SUMIF($D2:$D17, TRUE, $O2:$O17), "hh:mm:ss")</f>
+        <v>00:02:52</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -11476,7 +11517,13 @@
         <v>3.9351851851848751E-4</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>609</v>
+        <v>875</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
@@ -11520,9 +11567,17 @@
         <f t="shared" si="3"/>
         <v>5.6712962962962576E-4</v>
       </c>
-      <c r="P12" t="str">
-        <f>TEXT(SUM(O2:O18)/ROWS(O2:O18), "hh:mm:ss")</f>
-        <v>00:01:12</v>
+      <c r="P12">
+        <f>ROWS(D2:D17)</f>
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <f>COUNTIF(D2:D17, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <f>COUNTIF(D2:D17, TRUE)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
@@ -11611,6 +11666,15 @@
         <f t="shared" si="3"/>
         <v>3.8194444444450415E-4</v>
       </c>
+      <c r="P14" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q14" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="R14" s="28" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
@@ -11653,6 +11717,18 @@
         <f t="shared" si="3"/>
         <v>4.8611111111107608E-4</v>
       </c>
+      <c r="P15" s="29">
+        <f>P10/P12</f>
+        <v>5.8449074074074078E-4</v>
+      </c>
+      <c r="Q15" s="29">
+        <f>Q10/Q12</f>
+        <v>6.6919191919191916E-4</v>
+      </c>
+      <c r="R15" s="29">
+        <f>R10/R12</f>
+        <v>3.9814814814814818E-4</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
@@ -11748,37 +11824,39 @@
       <c r="C18" t="s">
         <v>276</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D18" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="H18" s="23">
+        <v>1</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="K18" s="6" t="str">
+      <c r="J18" s="23"/>
+      <c r="K18" s="23" t="str">
         <f t="shared" si="0"/>
         <v>2018-03-07</v>
       </c>
-      <c r="L18" s="9" t="str">
+      <c r="L18" s="24" t="str">
         <f t="shared" si="1"/>
         <v>11:57:12</v>
       </c>
-      <c r="N18" t="str">
+      <c r="M18" s="23"/>
+      <c r="N18" s="23" t="str">
         <f t="shared" si="2"/>
         <v>00:06:53</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="24">
         <f t="shared" si="3"/>
         <v>4.7800925925925442E-3</v>
       </c>
@@ -12217,7 +12295,7 @@
       </c>
       <c r="P32" s="9"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>42</v>
       </c>
@@ -12259,10 +12337,16 @@
         <v>8.796296296296191E-4</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>611</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R33" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -12303,12 +12387,20 @@
         <f t="shared" si="5"/>
         <v>2.083333333333659E-4</v>
       </c>
-      <c r="P34" t="str">
-        <f>TEXT(SUM(O24:O40)/ROWS(O24:O40), "hh:mm:ss")</f>
-        <v>00:00:34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P34" s="9" t="str">
+        <f>TEXT(SUM($O24:$O40), "hh:mm:ss")</f>
+        <v>00:09:30</v>
+      </c>
+      <c r="Q34" s="9" t="str">
+        <f>TEXT(SUMIF($D24:$D40, FALSE, $O24:$O40), "hh:mm:ss")</f>
+        <v>00:06:54</v>
+      </c>
+      <c r="R34" s="9" t="str">
+        <f>TEXT(SUMIF($D24:$D40, TRUE, $O24:$O40), "hh:mm:ss")</f>
+        <v>00:02:36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>39</v>
       </c>
@@ -12349,8 +12441,17 @@
         <f t="shared" si="5"/>
         <v>1.96759259259216E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P35" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q35" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R35" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>56</v>
       </c>
@@ -12391,8 +12492,20 @@
         <f t="shared" si="5"/>
         <v>1.3425925925926174E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="P36">
+        <f>ROWS(D24:D40)</f>
+        <v>17</v>
+      </c>
+      <c r="Q36">
+        <f>COUNTIF(D24:D40, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="R36">
+        <f>COUNTIF(D24:D40, TRUE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>596</v>
       </c>
@@ -12437,7 +12550,7 @@
         <v>2.3148148148144365E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>50</v>
       </c>
@@ -12478,8 +12591,18 @@
         <f t="shared" si="5"/>
         <v>2.4305555555553804E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P38" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q38" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="R38" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
@@ -12520,8 +12643,21 @@
         <f t="shared" si="5"/>
         <v>1.7361111111119376E-4</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P39" s="29">
+        <f>P34/P36</f>
+        <v>3.8807189542483658E-4</v>
+      </c>
+      <c r="Q39" s="29">
+        <f>Q34/Q36</f>
+        <v>4.3560606060606065E-4</v>
+      </c>
+      <c r="R39" s="29">
+        <f>R34/R36</f>
+        <v>3.0092592592592595E-4</v>
+      </c>
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>47</v>
       </c>
@@ -12563,10 +12699,10 @@
         <v>1.5046296296294948E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K41" s="6"/>
     </row>
-    <row r="42" spans="1:16" ht="87" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:19" ht="87" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>602</v>
       </c>
@@ -12603,7 +12739,7 @@
         <v>11:32:07</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>50</v>
       </c>
@@ -12645,7 +12781,7 @@
         <v>7.6388888888889728E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>53</v>
       </c>
@@ -12687,7 +12823,7 @@
         <v>4.1666666666667629E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
@@ -12732,7 +12868,7 @@
         <v>3.5879629629631538E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>187</v>
       </c>
@@ -12774,7 +12910,7 @@
         <v>1.8055555555555602E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>190</v>
       </c>
@@ -12816,7 +12952,7 @@
         <v>9.8379629629624654E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>607</v>
       </c>
@@ -12865,7 +13001,7 @@
       </c>
       <c r="P48" s="10"/>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>197</v>
       </c>
@@ -12908,7 +13044,7 @@
       </c>
       <c r="P49" s="10"/>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>200</v>
       </c>
@@ -12951,7 +13087,7 @@
       </c>
       <c r="P50" s="9"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>202</v>
       </c>
@@ -12993,10 +13129,16 @@
         <v>1.7361111111119376E-4</v>
       </c>
       <c r="P51" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.35">
+        <v>611</v>
+      </c>
+      <c r="Q51" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R51" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>204</v>
       </c>
@@ -13037,12 +13179,20 @@
         <f t="shared" si="7"/>
         <v>2.4305555555553804E-4</v>
       </c>
-      <c r="P52" t="str">
-        <f>TEXT(SUM(O43:O58)/ROWS(O43:O58), "hh:mm:ss")</f>
-        <v>00:01:05</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P52" s="9" t="str">
+        <f>TEXT(SUM($O43:$O58), "hh:mm:ss")</f>
+        <v>00:17:21</v>
+      </c>
+      <c r="Q52" s="9" t="str">
+        <f>TEXT(SUMIF($D43:$D58, FALSE, $O43:$O58), "hh:mm:ss")</f>
+        <v>00:05:17</v>
+      </c>
+      <c r="R52" s="9" t="str">
+        <f>TEXT(SUMIF($D43:$D58, TRUE, $O43:$O58), "hh:mm:ss")</f>
+        <v>00:12:04</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>206</v>
       </c>
@@ -13083,8 +13233,17 @@
         <f t="shared" si="7"/>
         <v>2.6620370370361579E-4</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P53" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q53" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R53" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>209</v>
       </c>
@@ -13125,8 +13284,20 @@
         <f t="shared" si="7"/>
         <v>2.4537037037037357E-3</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P54">
+        <f>ROWS(D43:D58)</f>
+        <v>16</v>
+      </c>
+      <c r="Q54">
+        <f>COUNTIF(D43:D58, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="R54">
+        <f>COUNTIF(D43:D58, TRUE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>106</v>
       </c>
@@ -13168,7 +13339,7 @@
         <v>5.0925925925926485E-4</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
@@ -13209,8 +13380,17 @@
         <f t="shared" si="7"/>
         <v>6.1342592592589229E-4</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P56" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q56" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="R56" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>113</v>
       </c>
@@ -13251,8 +13431,20 @@
         <f t="shared" si="7"/>
         <v>4.5138888888895945E-4</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P57" s="9">
+        <f>P52/P54</f>
+        <v>7.5303819444444452E-4</v>
+      </c>
+      <c r="Q57" s="9">
+        <f>Q52/Q54</f>
+        <v>7.337962962962963E-4</v>
+      </c>
+      <c r="R57" s="9">
+        <f>R52/R54</f>
+        <v>7.6178451178451174E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
         <v>115</v>
       </c>
@@ -13294,7 +13486,7 @@
         <v>1.1805555555555181E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -13305,7 +13497,7 @@
       <c r="I59" s="1"/>
       <c r="K59" s="6"/>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B60" s="1" t="s">
         <v>145</v>
       </c>
@@ -13339,7 +13531,7 @@
         <v>11:33:26</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B61" s="1" t="s">
         <v>149</v>
       </c>
@@ -13381,7 +13573,7 @@
         <v>7.523148148148584E-4</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
         <v>155</v>
       </c>
@@ -13423,7 +13615,7 @@
         <v>9.6064814814811328E-4</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
         <v>158</v>
       </c>
@@ -13465,7 +13657,7 @@
         <v>7.4074074074076401E-4</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>161</v>
       </c>
@@ -13507,7 +13699,7 @@
         <v>1.6666666666666496E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
         <v>604</v>
       </c>
@@ -13552,7 +13744,7 @@
         <v>4.9768518518522598E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>168</v>
       </c>
@@ -13595,7 +13787,7 @@
       </c>
       <c r="P66" s="10"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>172</v>
       </c>
@@ -13638,7 +13830,7 @@
       </c>
       <c r="P67" s="10"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>166</v>
       </c>
@@ -13681,7 +13873,7 @@
       </c>
       <c r="P68" s="9"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>170</v>
       </c>
@@ -13722,11 +13914,9 @@
         <f t="shared" si="9"/>
         <v>5.0925925925926485E-4</v>
       </c>
-      <c r="P69" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P69" s="10"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>175</v>
       </c>
@@ -13767,12 +13957,17 @@
         <f t="shared" si="9"/>
         <v>1.96759259259216E-4</v>
       </c>
-      <c r="P70" t="str">
-        <f>TEXT(SUM(O61:O77)/ROWS(O61:O77), "hh:mm:ss")</f>
-        <v>00:00:53</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P70" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q70" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R70" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>600</v>
       </c>
@@ -13816,8 +14011,20 @@
         <f t="shared" si="9"/>
         <v>1.0185185185185297E-3</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P71" s="9" t="str">
+        <f>TEXT(SUM($O61:$O77), "hh:mm:ss")</f>
+        <v>00:14:56</v>
+      </c>
+      <c r="Q71" s="9" t="str">
+        <f>TEXT(SUMIF($D61:$D77, FALSE, $O61:$O77), "hh:mm:ss")</f>
+        <v>00:04:33</v>
+      </c>
+      <c r="R71" s="9" t="str">
+        <f>TEXT(SUMIF($D61:$D77, TRUE, $O61:$O77), "hh:mm:ss")</f>
+        <v>00:10:23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B72" s="1" t="s">
         <v>250</v>
       </c>
@@ -13858,8 +14065,17 @@
         <f t="shared" si="9"/>
         <v>4.2824074074071516E-4</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P72" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q72" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R72" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>253</v>
       </c>
@@ -13900,8 +14116,20 @@
         <f t="shared" si="9"/>
         <v>2.1990740740740478E-4</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P73">
+        <f>ROWS(D61:D77)</f>
+        <v>17</v>
+      </c>
+      <c r="Q73">
+        <f>COUNTIF(D61:D77, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="R73">
+        <f>COUNTIF(D61:D77, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
         <v>261</v>
       </c>
@@ -13943,7 +14171,7 @@
         <v>5.7870370370416424E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B75" s="2" t="s">
         <v>258</v>
       </c>
@@ -13984,8 +14212,17 @@
         <f t="shared" si="9"/>
         <v>8.1018518518494176E-5</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P75" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q75" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="R75" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B76" s="2" t="s">
         <v>264</v>
       </c>
@@ -14026,8 +14263,20 @@
         <f t="shared" si="9"/>
         <v>1.388888888889106E-4</v>
       </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P76" s="9">
+        <f>P71/P73</f>
+        <v>6.1002178649237468E-4</v>
+      </c>
+      <c r="Q76" s="9">
+        <f>Q71/Q73</f>
+        <v>6.3194444444444442E-4</v>
+      </c>
+      <c r="R76" s="9">
+        <f>R71/R73</f>
+        <v>6.0088734567901225E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>247</v>
       </c>
@@ -14069,94 +14318,98 @@
         <v>1.0532407407407018E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>184</v>
       </c>
       <c r="C78" t="s">
         <v>184</v>
       </c>
-      <c r="D78" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="D78" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78" t="s">
+      <c r="H78" s="25">
+        <v>1</v>
+      </c>
+      <c r="I78" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="K78" s="6" t="str">
+      <c r="J78" s="25"/>
+      <c r="K78" s="25" t="str">
         <f t="shared" si="10"/>
         <v>2018-03-07</v>
       </c>
-      <c r="L78" s="9" t="str">
+      <c r="L78" s="26" t="str">
         <f t="shared" si="11"/>
         <v>14:53:33</v>
       </c>
-      <c r="N78" s="13" t="str">
+      <c r="M78" s="25"/>
+      <c r="N78" s="25" t="str">
         <f t="shared" si="8"/>
         <v>03:05:11</v>
       </c>
-      <c r="O78" s="14">
+      <c r="O78" s="26">
         <f t="shared" si="9"/>
         <v>0.12859953703703703</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>313</v>
       </c>
       <c r="C79" t="s">
         <v>313</v>
       </c>
-      <c r="D79" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="D79" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="H79">
-        <v>1</v>
-      </c>
-      <c r="I79" t="s">
+      <c r="H79" s="25">
+        <v>1</v>
+      </c>
+      <c r="I79" s="25" t="s">
         <v>315</v>
       </c>
-      <c r="K79" s="6" t="str">
+      <c r="J79" s="25"/>
+      <c r="K79" s="25" t="str">
         <f t="shared" si="10"/>
         <v>2018-03-07</v>
       </c>
-      <c r="L79" s="9" t="str">
+      <c r="L79" s="26" t="str">
         <f t="shared" si="11"/>
         <v>14:57:22</v>
       </c>
-      <c r="N79" s="13" t="str">
+      <c r="M79" s="25"/>
+      <c r="N79" s="25" t="str">
         <f t="shared" si="8"/>
         <v>00:03:49</v>
       </c>
-      <c r="O79" s="14">
+      <c r="O79" s="26">
         <f t="shared" si="9"/>
         <v>2.6504629629630072E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="K80" s="6"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>134</v>
       </c>
@@ -14187,7 +14440,7 @@
         <v>11:30:31</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>106</v>
       </c>
@@ -14229,7 +14482,7 @@
         <v>9.0277777777775237E-4</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>601</v>
       </c>
@@ -14274,7 +14527,7 @@
         <v>8.101851851851638E-4</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B84" s="1" t="s">
         <v>113</v>
       </c>
@@ -14316,7 +14569,7 @@
         <v>4.2824074074077068E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B85" s="1" t="s">
         <v>115</v>
       </c>
@@ -14358,7 +14611,7 @@
         <v>4.3981481481480955E-4</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>117</v>
       </c>
@@ -14400,7 +14653,7 @@
         <v>3.3564814814818211E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>119</v>
       </c>
@@ -14443,7 +14696,7 @@
       </c>
       <c r="P87" s="10"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>121</v>
       </c>
@@ -14486,7 +14739,7 @@
       </c>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>123</v>
       </c>
@@ -14529,7 +14782,7 @@
       </c>
       <c r="P89" s="9"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>128</v>
       </c>
@@ -14570,11 +14823,9 @@
         <f t="shared" si="13"/>
         <v>1.2847222222222565E-3</v>
       </c>
-      <c r="P90" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P90" s="10"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>130</v>
       </c>
@@ -14615,12 +14866,17 @@
         <f t="shared" si="13"/>
         <v>1.2731481481481621E-4</v>
       </c>
-      <c r="P91" t="str">
-        <f>TEXT(SUM(O82:O98)/ROWS(O82:O98), "hh:mm:ss")</f>
-        <v>00:00:49</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="P91" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q91" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R91" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>606</v>
       </c>
@@ -14664,8 +14920,20 @@
         <f t="shared" si="13"/>
         <v>6.4814814814817545E-4</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P92" s="9" t="str">
+        <f>TEXT(SUM($O82:$O98), "hh:mm:ss")</f>
+        <v>00:13:55</v>
+      </c>
+      <c r="Q92" s="9" t="str">
+        <f>TEXT(SUMIF($D82:$D98, FALSE, $O82:$O98), "hh:mm:ss")</f>
+        <v>00:11:22</v>
+      </c>
+      <c r="R92" s="9" t="str">
+        <f>TEXT(SUMIF($D82:$D98, TRUE, $O82:$O98), "hh:mm:ss")</f>
+        <v>00:02:33</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>132</v>
       </c>
@@ -14706,8 +14974,17 @@
         <f t="shared" si="13"/>
         <v>2.8935185185174905E-4</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P93" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q93" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R93" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>137</v>
       </c>
@@ -14748,8 +15025,20 @@
         <f t="shared" si="13"/>
         <v>6.3657407407413658E-4</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P94">
+        <f>ROWS(D82:D98)</f>
+        <v>17</v>
+      </c>
+      <c r="Q94">
+        <f>COUNTIF(D82:D98, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="R94">
+        <f>COUNTIF(D82:D98, TRUE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>599</v>
       </c>
@@ -14794,7 +15083,7 @@
         <v>7.407407407407085E-4</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A96" s="8" t="s">
         <v>598</v>
       </c>
@@ -14838,8 +15127,17 @@
         <f t="shared" si="13"/>
         <v>3.7037037037035425E-4</v>
       </c>
-    </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P96" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q96" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="R96" s="28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B97" s="1" t="s">
         <v>143</v>
       </c>
@@ -14880,8 +15178,20 @@
         <f t="shared" si="13"/>
         <v>4.0509259259263741E-4</v>
       </c>
-    </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P97" s="29">
+        <f>P92/P94</f>
+        <v>5.6849128540305011E-4</v>
+      </c>
+      <c r="Q97" s="29">
+        <f>Q92/Q94</f>
+        <v>6.5779320987654317E-4</v>
+      </c>
+      <c r="R97" s="29">
+        <f>R92/R94</f>
+        <v>3.5416666666666664E-4</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B98" s="5" t="s">
         <v>152</v>
       </c>
@@ -14923,7 +15233,7 @@
         <v>1.4583333333333393E-3</v>
       </c>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -14934,7 +15244,7 @@
       <c r="I99" s="5"/>
       <c r="K99" s="6"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B100" s="6" t="s">
         <v>139</v>
       </c>
@@ -14971,7 +15281,7 @@
         <v>11:37:13</v>
       </c>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B101" s="6" t="s">
         <v>141</v>
       </c>
@@ -15013,7 +15323,7 @@
         <v>1.3657407407407507E-3</v>
       </c>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B102" s="1" t="s">
         <v>143</v>
       </c>
@@ -15055,7 +15365,7 @@
         <v>4.9768518518517046E-4</v>
       </c>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B103" s="5" t="s">
         <v>152</v>
       </c>
@@ -15100,7 +15410,7 @@
         <v>1.3657407407408062E-3</v>
       </c>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>229</v>
       </c>
@@ -15142,7 +15452,7 @@
         <v>8.3333333333329707E-4</v>
       </c>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>232</v>
       </c>
@@ -15184,7 +15494,7 @@
         <v>4.3981481481480955E-4</v>
       </c>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>235</v>
       </c>
@@ -15226,7 +15536,7 @@
         <v>3.2407407407403221E-4</v>
       </c>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>238</v>
       </c>
@@ -15269,7 +15579,7 @@
       </c>
       <c r="P107" s="10"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>241</v>
       </c>
@@ -15312,7 +15622,7 @@
       </c>
       <c r="P108" s="10"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B109" s="2" t="s">
         <v>66</v>
       </c>
@@ -15355,7 +15665,7 @@
       </c>
       <c r="P109" s="9"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B110" s="1" t="s">
         <v>65</v>
       </c>
@@ -15397,10 +15707,16 @@
         <v>7.9861111111106942E-4</v>
       </c>
       <c r="P110" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.35">
+        <v>611</v>
+      </c>
+      <c r="Q110" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R110" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B111" s="1" t="s">
         <v>62</v>
       </c>
@@ -15441,12 +15757,20 @@
         <f t="shared" si="15"/>
         <v>2.662037037036713E-4</v>
       </c>
-      <c r="P111" t="str">
-        <f>TEXT(SUM(O101:O117)/ROWS(O101:O117), "hh:mm:ss")</f>
-        <v>00:00:58</v>
-      </c>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P111" s="9" t="str">
+        <f>TEXT(SUM($O101:$O117), "hh:mm:ss")</f>
+        <v>00:16:23</v>
+      </c>
+      <c r="Q111" s="9" t="str">
+        <f>TEXT(SUMIF($D101:$D117, FALSE, $O101:$O117), "hh:mm:ss")</f>
+        <v>00:01:50</v>
+      </c>
+      <c r="R111" s="9" t="str">
+        <f>TEXT(SUMIF($D101:$D117, TRUE, $O101:$O117), "hh:mm:ss")</f>
+        <v>00:14:33</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B112" s="1" t="s">
         <v>58</v>
       </c>
@@ -15487,8 +15811,17 @@
         <f t="shared" si="15"/>
         <v>1.6203703703709937E-4</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P112" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q112" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R112" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>355</v>
       </c>
@@ -15529,8 +15862,20 @@
         <f t="shared" si="15"/>
         <v>1.6203703703704386E-4</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P113">
+        <f>ROWS(D101:D117)</f>
+        <v>17</v>
+      </c>
+      <c r="Q113">
+        <f>COUNTIF(D101:D117, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="R113">
+        <f>COUNTIF(D101:D117, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>352</v>
       </c>
@@ -15572,7 +15917,7 @@
         <v>1.9675925925927151E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>349</v>
       </c>
@@ -15613,8 +15958,20 @@
         <f t="shared" si="15"/>
         <v>1.6203703703698835E-4</v>
       </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P115" s="27" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q115" s="27" t="s">
+        <v>609</v>
+      </c>
+      <c r="R115" s="27" t="s">
+        <v>609</v>
+      </c>
+      <c r="S115" s="27" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>346</v>
       </c>
@@ -15655,8 +16012,23 @@
         <f t="shared" si="15"/>
         <v>3.0092592592595446E-4</v>
       </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P116" s="24">
+        <f>P111/P113</f>
+        <v>6.6925381263616558E-4</v>
+      </c>
+      <c r="Q116" s="24">
+        <f>Q111/Q113</f>
+        <v>2.5462962962962966E-4</v>
+      </c>
+      <c r="R116" s="24">
+        <f>R111/R113</f>
+        <v>8.42013888888889E-4</v>
+      </c>
+      <c r="S116" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>343</v>
       </c>
@@ -15698,10 +16070,10 @@
         <v>4.5138888888884843E-4</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="K118" s="6"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B119" s="1" t="s">
         <v>58</v>
       </c>
@@ -15735,7 +16107,7 @@
         <v>11:32:41</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B120" s="1" t="s">
         <v>62</v>
       </c>
@@ -15777,7 +16149,7 @@
         <v>2.7777777777776569E-4</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="7" t="s">
         <v>597</v>
       </c>
@@ -15822,7 +16194,7 @@
         <v>6.94444444444553E-5</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>69</v>
       </c>
@@ -15864,7 +16236,7 @@
         <v>3.5879629629631538E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>71</v>
       </c>
@@ -15906,7 +16278,7 @@
         <v>1.1574074074066631E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>74</v>
       </c>
@@ -15948,7 +16320,7 @@
         <v>1.9675925925927151E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>76</v>
       </c>
@@ -15990,7 +16362,7 @@
         <v>2.6620370370372681E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>79</v>
       </c>
@@ -16033,7 +16405,7 @@
       </c>
       <c r="P126" s="10"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>82</v>
       </c>
@@ -16074,11 +16446,9 @@
         <f t="shared" si="17"/>
         <v>3.1249999999999334E-4</v>
       </c>
-      <c r="P127" s="10" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P127" s="10"/>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>84</v>
       </c>
@@ -16121,7 +16491,7 @@
       </c>
       <c r="P128" s="9"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>87</v>
       </c>
@@ -16163,10 +16533,16 @@
         <v>8.1018518518494176E-5</v>
       </c>
       <c r="P129" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
+        <v>611</v>
+      </c>
+      <c r="Q129" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R129" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>90</v>
       </c>
@@ -16207,12 +16583,20 @@
         <f t="shared" si="17"/>
         <v>2.3148148148155467E-4</v>
       </c>
-      <c r="P130" t="str">
-        <f>TEXT(SUM(O120:O136)/ROWS(O120:O136), "hh:mm:ss")</f>
-        <v>00:00:25</v>
-      </c>
-    </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P130" s="9" t="str">
+        <f>TEXT(SUM($O120:$O136), "hh:mm:ss")</f>
+        <v>00:07:05</v>
+      </c>
+      <c r="Q130" s="9" t="str">
+        <f>TEXT(SUMIF($D120:$D136, FALSE, $O120:$O136), "hh:mm:ss")</f>
+        <v>00:05:29</v>
+      </c>
+      <c r="R130" s="9" t="str">
+        <f>TEXT(SUMIF($D120:$D136, TRUE, $O120:$O136), "hh:mm:ss")</f>
+        <v>00:01:36</v>
+      </c>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>92</v>
       </c>
@@ -16253,8 +16637,17 @@
         <f t="shared" si="17"/>
         <v>1.1574074074072183E-4</v>
       </c>
-    </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P131" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q131" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R131" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B132" s="1" t="s">
         <v>94</v>
       </c>
@@ -16295,8 +16688,20 @@
         <f t="shared" si="17"/>
         <v>3.4722222222222099E-4</v>
       </c>
-    </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P132">
+        <f>ROWS(D120:D136)</f>
+        <v>17</v>
+      </c>
+      <c r="Q132">
+        <f>COUNTIF(D120:D136, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="R132">
+        <f>COUNTIF(D120:D136, TRUE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B133" s="1" t="s">
         <v>97</v>
       </c>
@@ -16338,7 +16743,7 @@
         <v>3.4722222222172139E-5</v>
       </c>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B134" s="1" t="s">
         <v>100</v>
       </c>
@@ -16379,8 +16784,17 @@
         <f t="shared" si="17"/>
         <v>3.472222222222765E-4</v>
       </c>
-    </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P134" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q134" s="28" t="s">
+        <v>609</v>
+      </c>
+      <c r="R134" s="28" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
         <v>102</v>
       </c>
@@ -16424,8 +16838,20 @@
         <f t="shared" si="17"/>
         <v>5.6712962962962576E-4</v>
       </c>
-    </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P135" s="29">
+        <f>P130/P132</f>
+        <v>2.8935185185185184E-4</v>
+      </c>
+      <c r="Q135" s="29">
+        <f>Q130/Q132</f>
+        <v>3.1732253086419758E-4</v>
+      </c>
+      <c r="R135" s="29">
+        <f>R130/R132</f>
+        <v>2.2222222222222223E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B136" s="1" t="s">
         <v>65</v>
       </c>
@@ -16467,7 +16893,7 @@
         <v>7.7546296296299166E-4</v>
       </c>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -16478,7 +16904,7 @@
       <c r="I137" s="1"/>
       <c r="K137" s="6"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B138" s="1" t="s">
         <v>97</v>
       </c>
@@ -16512,7 +16938,7 @@
         <v>11:42:35</v>
       </c>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B139" s="1" t="s">
         <v>100</v>
       </c>
@@ -16554,7 +16980,7 @@
         <v>2.8935185185186008E-4</v>
       </c>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B140" s="1" t="s">
         <v>94</v>
       </c>
@@ -16596,7 +17022,7 @@
         <v>2.1990740740740478E-4</v>
       </c>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B141" s="1" t="s">
         <v>102</v>
       </c>
@@ -16641,7 +17067,7 @@
         <v>4.1666666666667629E-4</v>
       </c>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>279</v>
       </c>
@@ -16683,7 +17109,7 @@
         <v>1.7245370370370661E-3</v>
       </c>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>295</v>
       </c>
@@ -16725,7 +17151,7 @@
         <v>2.1990740740740478E-4</v>
       </c>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>282</v>
       </c>
@@ -16770,7 +17196,7 @@
         <v>2.8935185185186008E-4</v>
       </c>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>289</v>
       </c>
@@ -16813,7 +17239,7 @@
       </c>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>298</v>
       </c>
@@ -16856,7 +17282,7 @@
       </c>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>303</v>
       </c>
@@ -16897,9 +17323,17 @@
         <f t="shared" si="21"/>
         <v>4.3981481481480955E-4</v>
       </c>
-      <c r="P147" s="9"/>
-    </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P147" s="10" t="s">
+        <v>611</v>
+      </c>
+      <c r="Q147" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="R147" s="10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="148" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>306</v>
       </c>
@@ -16940,11 +17374,20 @@
         <f t="shared" si="21"/>
         <v>1.1574074074077734E-4</v>
       </c>
-      <c r="P148" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P148" s="9" t="str">
+        <f>TEXT(SUM($O139:$O154), "hh:mm:ss")</f>
+        <v>00:09:52</v>
+      </c>
+      <c r="Q148" s="9" t="str">
+        <f>TEXT(SUMIF($D139:$D154, FALSE, $O139:$O154), "hh:mm:ss")</f>
+        <v>00:02:48</v>
+      </c>
+      <c r="R148" s="9" t="str">
+        <f>TEXT(SUMIF($D139:$D154, TRUE, $O139:$O154), "hh:mm:ss")</f>
+        <v>00:07:04</v>
+      </c>
+    </row>
+    <row r="149" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>309</v>
       </c>
@@ -16988,12 +17431,17 @@
         <f t="shared" si="21"/>
         <v>5.5555555555553138E-4</v>
       </c>
-      <c r="P149" t="str">
-        <f>TEXT(SUM(O139:O154)/ROWS(O139:O154), "hh:mm:ss")</f>
-        <v>00:00:37</v>
-      </c>
-    </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P149" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q149" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="R149" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="150" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>316</v>
       </c>
@@ -17037,8 +17485,20 @@
         <f t="shared" si="21"/>
         <v>8.3333333333335258E-4</v>
       </c>
-    </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P150">
+        <f>ROWS(D139:D154)</f>
+        <v>16</v>
+      </c>
+      <c r="Q150">
+        <f>COUNTIF(D139:D154, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="R150">
+        <f>COUNTIF(D139:D154, TRUE)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B151" s="1" t="s">
         <v>145</v>
       </c>
@@ -17080,7 +17540,7 @@
         <v>1.8518518518512161E-4</v>
       </c>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B152" s="1" t="s">
         <v>149</v>
       </c>
@@ -17121,8 +17581,17 @@
         <f t="shared" si="21"/>
         <v>1.6203703703704386E-4</v>
       </c>
-    </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P152" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q152" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="R152" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="153" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B153" s="5" t="s">
         <v>155</v>
       </c>
@@ -17166,8 +17635,20 @@
         <f t="shared" si="21"/>
         <v>5.3240740740745363E-4</v>
       </c>
-    </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P153" s="9">
+        <f>P148/P150</f>
+        <v>4.2824074074074075E-4</v>
+      </c>
+      <c r="Q153" s="9">
+        <f>Q148/Q150</f>
+        <v>4.8611111111111104E-4</v>
+      </c>
+      <c r="R153" s="9">
+        <f>R148/R150</f>
+        <v>4.0895061728395062E-4</v>
+      </c>
+    </row>
+    <row r="154" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B154" s="5" t="s">
         <v>158</v>
       </c>
@@ -17219,7 +17700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="R150" sqref="R150"/>
     </sheetView>
   </sheetViews>
@@ -23246,7 +23727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView topLeftCell="F13" workbookViewId="0">
+    <sheetView topLeftCell="F78" workbookViewId="0">
       <selection activeCell="P11" sqref="P11:P12"/>
     </sheetView>
   </sheetViews>
@@ -29495,8 +29976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="G185" sqref="G185"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>